<commit_message>
predicted my mape method on the test data
</commit_message>
<xml_diff>
--- a/data/labeled_claims/population_claims.xlsx
+++ b/data/labeled_claims/population_claims.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
+  <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhruv/Documents/university/ClaimDetection/data/labeled_claims/"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11092" uniqueCount="2791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11097" uniqueCount="2796">
   <si>
     <t>&lt;location&gt;Cambodia&lt;/location&gt; has an estimated population of &lt;number&gt;13 million&lt;/number&gt; -LRB- 2004 estimate -RRB- , with a labor participation rate of 72 percent .</t>
   </si>
@@ -8400,6 +8400,21 @@
   </si>
   <si>
     <t>extracted_value</t>
+  </si>
+  <si>
+    <t>sentence</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>mape_support</t>
+  </si>
+  <si>
+    <t>pattern</t>
   </si>
 </sst>
 </file>
@@ -8852,8 +8867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1586"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="C457" sqref="C457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8861,19 +8876,34 @@
     <col min="3" max="3" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2792</v>
+      </c>
       <c r="B1" t="s">
         <v>2786</v>
       </c>
+      <c r="C1" t="s">
+        <v>2791</v>
+      </c>
       <c r="D1" t="s">
         <v>2787</v>
       </c>
       <c r="E1" t="s">
         <v>2788</v>
       </c>
+      <c r="F1" t="s">
+        <v>2793</v>
+      </c>
       <c r="G1" t="s">
         <v>2789</v>
       </c>
+      <c r="H1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2795</v>
+      </c>
       <c r="J1" t="s">
         <v>2790</v>
       </c>
@@ -8881,7 +8911,7 @@
         <v>2785</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2780</v>
       </c>
@@ -8916,7 +8946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2781</v>
       </c>
@@ -8951,7 +8981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2781</v>
       </c>
@@ -8986,7 +9016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2780</v>
       </c>
@@ -9021,7 +9051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2780</v>
       </c>
@@ -9056,7 +9086,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>2780</v>
       </c>
@@ -9091,7 +9121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>2780</v>
       </c>
@@ -9126,7 +9156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>2780</v>
       </c>
@@ -9161,7 +9191,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>2780</v>
       </c>
@@ -9196,7 +9226,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>2780</v>
       </c>
@@ -9231,7 +9261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>2780</v>
       </c>
@@ -9266,7 +9296,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>2780</v>
       </c>
@@ -9301,7 +9331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>2780</v>
       </c>
@@ -9336,7 +9366,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>2780</v>
       </c>
@@ -9371,7 +9401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>2780</v>
       </c>

</xml_diff>